<commit_message>
Updated completed states, updated JSON objects
</commit_message>
<xml_diff>
--- a/CompletedStates.xlsx
+++ b/CompletedStates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="55">
   <si>
     <t xml:space="preserve">Alabama </t>
   </si>
@@ -125,9 +125,6 @@
     <t xml:space="preserve">Oregon </t>
   </si>
   <si>
-    <t xml:space="preserve">Pennsylvania Rhode Island </t>
-  </si>
-  <si>
     <t xml:space="preserve">South Carolina </t>
   </si>
   <si>
@@ -183,16 +180,32 @@
   </si>
   <si>
     <t xml:space="preserve">Montana  </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pennsylvania </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhode Island </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,8 +231,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,13 +525,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -524,99 +539,153 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,10 +693,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -635,18 +704,21 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -654,10 +726,10 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -665,26 +737,32 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -692,10 +770,10 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -703,10 +781,10 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -714,28 +792,43 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -743,10 +836,10 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -754,146 +847,241 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>25</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>26</v>
       </c>
+      <c r="B32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>27</v>
       </c>
+      <c r="B33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>28</v>
       </c>
+      <c r="B34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>29</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>30</v>
       </c>
+      <c r="B36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>53</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" t="s">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" t="s">
-        <v>46</v>
+        <v>37</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>44</v>
+      <c r="B51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>